<commit_message>
Pdf file to explain csv files is added
</commit_message>
<xml_diff>
--- a/Config_Opt.xlsx
+++ b/Config_Opt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szata\Codes\StoriesTeams\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D548789B-9072-459B-BFF4-F8B2CA125F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48881C1E-EAA0-4B3F-8DCD-D5C2E5C58191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -230,10 +230,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -501,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -650,7 +646,7 @@
         <v>11</v>
       </c>
       <c r="D10" s="1">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -664,7 +660,7 @@
         <v>12</v>
       </c>
       <c r="D11" s="1">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1002,7 +998,7 @@
         <v>11</v>
       </c>
       <c r="D35" s="1">
-        <v>80</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1016,7 +1012,7 @@
         <v>12</v>
       </c>
       <c r="D36" s="1">
-        <v>80</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Timeseries folder, readme update
</commit_message>
<xml_diff>
--- a/Config_Opt.xlsx
+++ b/Config_Opt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szata\Codes\StoriesTeams\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171751B8-E418-4EDE-A563-D8A3ABE5CA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EED013-B51F-4262-A5E0-321AE463EC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,7 +189,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -211,11 +211,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43:C47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,572 +513,572 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="4">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="3">
         <v>10000000000000</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="3">
         <v>10000000000000</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="3">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="A8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="3">
         <v>3.41</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="3">
         <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="3">
         <v>0.95</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="3">
         <v>0.95</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="3">
         <v>28700</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="3">
         <v>0.8</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="3">
         <v>0.2</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="A16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="3">
         <v>2E-3</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="A17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="3">
         <v>100000</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="A18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="A19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="3">
         <v>0.9</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="3">
         <v>0.9</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="A21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="A22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="3">
         <v>0.8</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="A23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="3">
         <v>0.2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="A24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="A25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="3">
         <v>57225</v>
       </c>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="A26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="3">
         <v>286.25</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="A27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="3">
         <v>0.65</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="A28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="3">
         <v>0.65</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="A29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="A30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="3">
         <v>0.8</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="A31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="3">
         <v>0.2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="A32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="3">
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="3">
         <v>17015</v>
       </c>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" s="3">
         <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="3">
         <v>0.8</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="3">
         <v>0.8</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="3">
         <v>0.8</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39" s="3">
         <v>0.2</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D40" s="3">
         <v>6.1500000000000001E-3</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -1087,198 +1089,198 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="A42" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42" s="3">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D43" s="3">
         <v>0.38</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>0</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="A44" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D44" s="3">
         <v>0.20200000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="A45" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D45" s="3">
         <v>0.35399999999999998</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>0</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="A46" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D46" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" t="s">
+      <c r="A47" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D47" s="3">
         <v>0.5</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="A48" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D48" s="3">
         <v>0.01</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="A49" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D49" s="3">
         <v>6000000</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="A50" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D50" s="3">
         <v>1.2E-2</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="A51" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D51" s="3">
         <v>6250000</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="A52" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D52" s="3">
         <v>2000000</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="A53" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D53" s="1">
+      <c r="D53" s="3">
         <v>0.01</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="A54" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D54" s="3">
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="A55" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D55" s="1">
+      <c r="D55" s="3">
         <v>150000</v>
       </c>
     </row>

</xml_diff>